<commit_message>
add metrics viusalization and save the metrics result in excel
</commit_message>
<xml_diff>
--- a/code/sampling_methods_analysis.xlsx
+++ b/code/sampling_methods_analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SS2023\MasterThesis\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{850EFBC4-ECCF-4092-8767-2BDF1DFFFF01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D763AC7F-BEB7-40BB-83C9-BD50340544F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4542,8 +4542,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="I38" sqref="I38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>